<commit_message>
docs : Start Plan Week 1
</commit_message>
<xml_diff>
--- a/Documents/Plan.xlsx
+++ b/Documents/Plan.xlsx
@@ -1,36 +1,116 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\huyqu\Documents\CodingStar\Soc Market\_N06-PTTKPM_Nhom11\Documents\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48DFBFF7-D026-422E-B2BB-E8ABA1AEA38B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="120" windowWidth="16155" windowHeight="8505"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Week 1" sheetId="1" r:id="rId1"/>
+    <sheet name="Week 2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="19">
+  <si>
+    <t>Thành viên</t>
+  </si>
+  <si>
+    <t>Công việc</t>
+  </si>
+  <si>
+    <t>Tiến độ</t>
+  </si>
+  <si>
+    <t>Kết quả</t>
+  </si>
+  <si>
+    <t>Đặng Đức Huy</t>
+  </si>
+  <si>
+    <t>Xác định đối tượng phục vụ và nhóm đối tượng liên quan</t>
+  </si>
+  <si>
+    <t>Phân loại các nhóm</t>
+  </si>
+  <si>
+    <t>Hoàng Thị Thảo Nhi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nguyễn Hoài Nam </t>
+  </si>
+  <si>
+    <t>Phân rã chức năng và kịch bản sử dụng</t>
+  </si>
+  <si>
+    <t>Thiết kế frontend: Giao diện Trang chủ</t>
+  </si>
+  <si>
+    <t>Vẽ bản phác thảo  sketch sơ bộ đầu tiên về chương trình. ( Trang chủ, Giỏ hàng )</t>
+  </si>
+  <si>
+    <t>Mô hình hóa hệ thống</t>
+  </si>
+  <si>
+    <t>Định nghĩa input và output</t>
+  </si>
+  <si>
+    <t>Thiết kế cơ sở dữ liệu: Bảng sản phẩm, người dùng, đơn hàng, danh mục.</t>
+  </si>
+  <si>
+    <t>Thiết kế sơ đồ kiến trúc hệ thống (frontend, backend, database)</t>
+  </si>
+  <si>
+    <t>Deadline</t>
+  </si>
+  <si>
+    <t>22/12</t>
+  </si>
+  <si>
+    <t>19/12</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
-      <name val="宋体"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -52,30 +132,42 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  </cellStyleXfs>
+  <cellXfs count="6">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-  </cellStyleXfs>
-  <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -149,7 +241,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -184,7 +275,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -360,45 +450,168 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
-  <sheetData/>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="33.85546875" customWidth="1"/>
+    <col min="2" max="2" width="73.140625" customWidth="1"/>
+    <col min="3" max="3" width="26.42578125" customWidth="1"/>
+    <col min="4" max="4" width="35.5703125" customWidth="1"/>
+    <col min="5" max="5" width="32" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="2"/>
+      <c r="E5" s="3"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="2"/>
+      <c r="E6" s="3"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="3"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="3"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="3"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="3"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+    </row>
+  </sheetData>
+  <mergeCells count="9">
+    <mergeCell ref="E2:E4"/>
+    <mergeCell ref="E5:E7"/>
+    <mergeCell ref="E8:E10"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="C2:C4"/>
+    <mergeCell ref="D2:D4"/>
+    <mergeCell ref="D5:D7"/>
+    <mergeCell ref="C8:C10"/>
+    <mergeCell ref="D8:D10"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
-  <sheetData/>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
-  <sheetData/>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
docs : Plan Week 2
</commit_message>
<xml_diff>
--- a/Documents/Plan.xlsx
+++ b/Documents/Plan.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\huyqu\Documents\CodingStar\Soc Market\_N06-PTTKPM_Nhom11\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48DFBFF7-D026-422E-B2BB-E8ABA1AEA38B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F66BF6C-D31C-4C8F-8C21-668D896C6A56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Week 1" sheetId="1" r:id="rId1"/>
-    <sheet name="Week 2" sheetId="2" r:id="rId2"/>
+    <sheet name="Week 2" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="27">
   <si>
     <t>Thành viên</t>
   </si>
@@ -91,6 +91,30 @@
   </si>
   <si>
     <t>19/12</t>
+  </si>
+  <si>
+    <t>17/12</t>
+  </si>
+  <si>
+    <t>Thiết kế Proposal</t>
+  </si>
+  <si>
+    <t>Lựa chọn mô hình phân tích phần mềm</t>
+  </si>
+  <si>
+    <t>Hướng sử dụng của dự án, đối tượng sử dụng và chức năng chính cung cấp</t>
+  </si>
+  <si>
+    <t>Hoàn thành tài liệu mô tả Use case</t>
+  </si>
+  <si>
+    <t>Đặc tả hệ thống ( kèm theo các hình vẽ mô tả )</t>
+  </si>
+  <si>
+    <t>26/12</t>
+  </si>
+  <si>
+    <t>Thể hiện ý tưởng của nhóm trong Proposal</t>
   </si>
 </sst>
 </file>
@@ -134,11 +158,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -148,7 +169,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -453,8 +482,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -467,50 +496,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="A2" t="s">
         <v>7</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -522,26 +551,26 @@
       <c r="C5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="2"/>
-      <c r="E5" s="3"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="4"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="2"/>
-      <c r="E6" s="3"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="4"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="3"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="3"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="4"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -550,27 +579,29 @@
       <c r="B8" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="3"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="3"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
+      <c r="C10" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -581,8 +612,8 @@
     <mergeCell ref="C2:C4"/>
     <mergeCell ref="D2:D4"/>
     <mergeCell ref="D5:D7"/>
-    <mergeCell ref="C8:C10"/>
     <mergeCell ref="D8:D10"/>
+    <mergeCell ref="C8:C9"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -590,28 +621,130 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C088904-3D48-4E5A-A778-B9A8FB72912F}">
+  <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="33.85546875" customWidth="1"/>
+    <col min="2" max="2" width="73.140625" customWidth="1"/>
+    <col min="3" max="3" width="26.42578125" customWidth="1"/>
+    <col min="4" max="4" width="35.5703125" customWidth="1"/>
+    <col min="5" max="5" width="32" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" s="3" t="s">
         <v>3</v>
       </c>
     </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C4" s="6"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" s="5"/>
+      <c r="E5" s="4"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="4"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="4"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C7" s="6"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="4"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="4"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C10" s="6"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+    </row>
   </sheetData>
+  <mergeCells count="9">
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:D10"/>
+    <mergeCell ref="E8:E10"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D2:D4"/>
+    <mergeCell ref="E2:E4"/>
+    <mergeCell ref="D5:D7"/>
+    <mergeCell ref="E5:E7"/>
+  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat: Update footer layout and add jQuery and Bootstrap scripts
</commit_message>
<xml_diff>
--- a/Documents/Plan.xlsx
+++ b/Documents/Plan.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\huyqu\Documents\CodingStar\Soc Market\_N06-PTTKPM_Nhom11\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thoai\Documents\PTKTPM\_N06-PTTKPM_Nhom11\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48DFBFF7-D026-422E-B2BB-E8ABA1AEA38B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42EF12B5-13F7-4E52-B776-E728B4261D38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Week 1" sheetId="1" r:id="rId1"/>
@@ -60,9 +60,6 @@
     <t>Hoàng Thị Thảo Nhi</t>
   </si>
   <si>
-    <t xml:space="preserve">Nguyễn Hoài Nam </t>
-  </si>
-  <si>
     <t>Phân rã chức năng và kịch bản sử dụng</t>
   </si>
   <si>
@@ -91,6 +88,9 @@
   </si>
   <si>
     <t>19/12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trịnh Hoài Nam </t>
   </si>
 </sst>
 </file>
@@ -101,7 +101,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -109,7 +109,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -134,21 +134,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -454,44 +453,44 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.85546875" customWidth="1"/>
-    <col min="2" max="2" width="73.140625" customWidth="1"/>
-    <col min="3" max="3" width="26.42578125" customWidth="1"/>
-    <col min="4" max="4" width="35.5703125" customWidth="1"/>
+    <col min="1" max="1" width="33.8984375" customWidth="1"/>
+    <col min="2" max="2" width="73.09765625" customWidth="1"/>
+    <col min="3" max="3" width="26.3984375" customWidth="1"/>
+    <col min="4" max="4" width="35.59765625" customWidth="1"/>
     <col min="5" max="5" width="32" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D1" s="4" t="s">
+      <c r="C1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="A2" t="s">
         <v>7</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
@@ -506,7 +505,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
@@ -514,33 +513,33 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" s="2"/>
+        <v>16</v>
+      </c>
+      <c r="D5" s="4"/>
       <c r="E5" s="3"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6" s="2"/>
+        <v>17</v>
+      </c>
+      <c r="D6" s="4"/>
       <c r="E6" s="3"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C7" s="3"/>
-      <c r="D7" s="2"/>
+      <c r="D7" s="4"/>
       <c r="E7" s="3"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -548,29 +547,29 @@
         <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
+        <v>16</v>
+      </c>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C9" s="3"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C10" s="3"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -595,7 +594,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">

</xml_diff>

<commit_message>
docs : Plan Week 3
</commit_message>
<xml_diff>
--- a/Documents/Plan.xlsx
+++ b/Documents/Plan.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\huyqu\Documents\CodingStar\Soc Market\_N06-PTTKPM_Nhom11\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F66BF6C-D31C-4C8F-8C21-668D896C6A56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{044D9EA9-6D32-433D-A387-338B79B9B066}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Week 1" sheetId="1" r:id="rId1"/>
     <sheet name="Week 2" sheetId="3" r:id="rId2"/>
+    <sheet name="Week 3" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="33">
   <si>
     <t>Thành viên</t>
   </si>
@@ -115,6 +116,24 @@
   </si>
   <si>
     <t>Thể hiện ý tưởng của nhóm trong Proposal</t>
+  </si>
+  <si>
+    <t>Liên kết với Cơ sở quản trị dữ liệu MongoDB</t>
+  </si>
+  <si>
+    <t>Phân tích và xây dựng mô hình xử lý DFD – các cấp của mô hình xử lý, sơ đồ hệ thống con của quy trình</t>
+  </si>
+  <si>
+    <t>Hoàn thiện Giao Diện trang chủ</t>
+  </si>
+  <si>
+    <t>Xây dựng mô hình dữ liệu (ER), phân tích quan hệ dữ liệu, chuyển đổi mô hình dữ liệu</t>
+  </si>
+  <si>
+    <t>Tạo 4 Model : User, Product, Order, OrderDetails</t>
+  </si>
+  <si>
+    <t>Xây dựng mô hình tựa Merise</t>
   </si>
 </sst>
 </file>
@@ -158,7 +177,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -170,13 +189,16 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -519,27 +541,27 @@
       <c r="B2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -551,26 +573,26 @@
       <c r="C5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="5"/>
-      <c r="E5" s="4"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="5"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="5"/>
-      <c r="E6" s="4"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="5"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="4"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="4"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="5"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -579,19 +601,19 @@
       <c r="B8" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="4"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
@@ -600,8 +622,8 @@
       <c r="C10" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -624,8 +646,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C088904-3D48-4E5A-A778-B9A8FB72912F}">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -661,24 +683,24 @@
       <c r="B2" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C4" s="6"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -687,24 +709,24 @@
       <c r="B5" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="D5" s="5"/>
-      <c r="E5" s="4"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="5"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="4"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="4"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="5"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C7" s="6"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="5"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -713,24 +735,24 @@
       <c r="B8" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="4"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C10" s="6"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -747,4 +769,133 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E481A053-4594-4494-95AF-B43D28385E87}">
+  <dimension ref="A1:E10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="33.85546875" customWidth="1"/>
+    <col min="2" max="2" width="90" customWidth="1"/>
+    <col min="3" max="3" width="26.42578125" customWidth="1"/>
+    <col min="4" max="4" width="35.5703125" customWidth="1"/>
+    <col min="5" max="5" width="32" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="7">
+        <v>45660</v>
+      </c>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C4" s="4"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="7">
+        <v>45660</v>
+      </c>
+      <c r="D5" s="6"/>
+      <c r="E5" s="5"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" s="5"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="5"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C7" s="4"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="5"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="7">
+        <v>45660</v>
+      </c>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" s="7"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="7"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+    </row>
+  </sheetData>
+  <mergeCells count="9">
+    <mergeCell ref="D8:D10"/>
+    <mergeCell ref="E8:E10"/>
+    <mergeCell ref="C8:C10"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D4"/>
+    <mergeCell ref="E2:E4"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:D7"/>
+    <mergeCell ref="E5:E7"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>